<commit_message>
fix space usage output file name bug
</commit_message>
<xml_diff>
--- a/result/ycsb-report.xlsx
+++ b/result/ycsb-report.xlsx
@@ -14,24 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>art</t>
-  </si>
-  <si>
-    <t>clht</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>combotree</t>
-  </si>
-  <si>
-    <t>fastfair</t>
-  </si>
-  <si>
-    <t>levelhash</t>
-  </si>
-  <si>
-    <t>masstree</t>
   </si>
 </sst>
 </file>
@@ -364,7 +349,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -372,31 +357,31 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>8</v>
+      </c>
+      <c r="F1">
         <v>16</v>
       </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
+      <c r="G1">
         <v>24</v>
       </c>
-      <c r="E1">
-        <v>2</v>
-      </c>
-      <c r="F1">
+      <c r="H1">
         <v>32</v>
       </c>
-      <c r="G1">
+      <c r="I1">
         <v>40</v>
       </c>
-      <c r="H1">
+      <c r="J1">
         <v>48</v>
-      </c>
-      <c r="I1">
-        <v>4</v>
-      </c>
-      <c r="J1">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -404,294 +389,31 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>3.38587</v>
+        <v>0.799024</v>
       </c>
       <c r="C2">
-        <v>0.351131</v>
+        <v>1.569348</v>
       </c>
       <c r="D2">
-        <v>3.466486</v>
+        <v>3.060714</v>
       </c>
       <c r="E2">
-        <v>0.66859</v>
+        <v>5.782971</v>
       </c>
       <c r="F2">
-        <v>3.245097</v>
+        <v>10.184222</v>
       </c>
       <c r="G2">
-        <v>2.773464</v>
+        <v>13.479196</v>
       </c>
       <c r="H2">
-        <v>2.857729</v>
+        <v>15.040625</v>
       </c>
       <c r="I2">
-        <v>1.23877</v>
+        <v>15.559625</v>
       </c>
       <c r="J2">
-        <v>2.190412</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="B3">
-        <v>16</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>24</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>32</v>
-      </c>
-      <c r="G3">
-        <v>40</v>
-      </c>
-      <c r="H3">
-        <v>48</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>7.100719</v>
-      </c>
-      <c r="C4">
-        <v>0.615471</v>
-      </c>
-      <c r="D4">
-        <v>6.379052</v>
-      </c>
-      <c r="E4">
-        <v>1.204831</v>
-      </c>
-      <c r="F4">
-        <v>6.109027</v>
-      </c>
-      <c r="G4">
-        <v>5.82418</v>
-      </c>
-      <c r="H4">
-        <v>5.677892</v>
-      </c>
-      <c r="I4">
-        <v>2.329924</v>
-      </c>
-      <c r="J4">
-        <v>4.380238</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>8</v>
-      </c>
-      <c r="F5">
-        <v>16</v>
-      </c>
-      <c r="G5">
-        <v>24</v>
-      </c>
-      <c r="H5">
-        <v>32</v>
-      </c>
-      <c r="I5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>0.437297</v>
-      </c>
-      <c r="C6">
-        <v>0.832026</v>
-      </c>
-      <c r="D6">
-        <v>1.525311</v>
-      </c>
-      <c r="E6">
-        <v>2.844114</v>
-      </c>
-      <c r="F6">
-        <v>4.36913</v>
-      </c>
-      <c r="G6">
-        <v>4.693989</v>
-      </c>
-      <c r="H6">
-        <v>5.842726</v>
-      </c>
-      <c r="I6">
-        <v>6.408001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="B7">
-        <v>16</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>24</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>40</v>
-      </c>
-      <c r="G7">
-        <v>48</v>
-      </c>
-      <c r="H7">
-        <v>4</v>
-      </c>
-      <c r="I7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>2.044068</v>
-      </c>
-      <c r="C8">
-        <v>0.139184</v>
-      </c>
-      <c r="D8">
-        <v>2.487764</v>
-      </c>
-      <c r="E8">
-        <v>0.282028</v>
-      </c>
-      <c r="F8">
-        <v>2.339656</v>
-      </c>
-      <c r="G8">
-        <v>2.245025</v>
-      </c>
-      <c r="H8">
-        <v>0.567119</v>
-      </c>
-      <c r="I8">
-        <v>1.116075</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="B9">
-        <v>16</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10">
-        <v>6877.579092</v>
-      </c>
-      <c r="C10">
-        <v>446.388715</v>
-      </c>
-      <c r="D10">
-        <v>892.936869</v>
-      </c>
-      <c r="E10">
-        <v>1780.9439</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="B11">
-        <v>16</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>24</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>32</v>
-      </c>
-      <c r="G11">
-        <v>40</v>
-      </c>
-      <c r="H11">
-        <v>48</v>
-      </c>
-      <c r="I11">
-        <v>4</v>
-      </c>
-      <c r="J11">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>3.540919</v>
-      </c>
-      <c r="C12">
-        <v>0.298118</v>
-      </c>
-      <c r="D12">
-        <v>4.40728</v>
-      </c>
-      <c r="E12">
-        <v>0.587493</v>
-      </c>
-      <c r="F12">
-        <v>4.673129</v>
-      </c>
-      <c r="G12">
-        <v>4.709541</v>
-      </c>
-      <c r="H12">
-        <v>4.468275</v>
-      </c>
-      <c r="I12">
-        <v>1.124152</v>
-      </c>
-      <c r="J12">
-        <v>2.062205</v>
+        <v>16.681012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>